<commit_message>
Matriz de Responsabilidades - Versión Final
</commit_message>
<xml_diff>
--- a/Documentos/Matriz de Responsabilidades PM.xlsx
+++ b/Documentos/Matriz de Responsabilidades PM.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="507"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="507"/>
   </bookViews>
   <sheets>
     <sheet name="Matriz de Responsabilidades" sheetId="1" r:id="rId1"/>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="106">
   <si>
     <t>Project Manager</t>
   </si>
@@ -472,9 +477,6 @@
     <t>Micaela Paredes</t>
   </si>
   <si>
-    <t>Nicolás Villalba</t>
-  </si>
-  <si>
     <t>Analía Revolero</t>
   </si>
   <si>
@@ -484,7 +486,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1078,7 +1080,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1089,10 +1091,10 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="L6" sqref="L6"/>
+      <selection pane="bottomRight" activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1203,19 +1205,19 @@
         <v>103</v>
       </c>
       <c r="E5" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="G5" s="8" t="s">
         <v>105</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>106</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>103</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="251.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1319,7 +1321,7 @@
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
     </row>
-    <row r="11" spans="1:9" ht="99.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="85.5" x14ac:dyDescent="0.2">
       <c r="B11" s="13" t="s">
         <v>8</v>
       </c>

</xml_diff>